<commit_message>
Checks for empty data
- added checks for empty dataframe after various filtering operations
- add doc for calibLThresh
- update config file format
- removed csv config file
</commit_message>
<xml_diff>
--- a/inst/extdata/geolocation_settings.xlsx
+++ b/inst/extdata/geolocation_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://007gc-my.sharepoint.com/personal/dave_fifield_ec_gc_ca/Documents/Papers and Presentations/GLS analysis session Dec 2023/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://007gc-my.sharepoint.com/personal/dave_fifield_ec_gc_ca/Documents/Projects/GLSHelper/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{3D8C0B10-F562-462F-936E-5D22F674CFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5F71A6BA-88F1-4CDF-9FE1-5A2C26365AD1}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="6_{7BDDE644-5E0F-4C9F-A1B7-CFDF8F32052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30B0B5E1-7040-4890-A57F-F4D19364DC4C}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t>tagName</t>
   </si>
@@ -103,9 +103,6 @@
     <t>calibAsk</t>
   </si>
   <si>
-    <t>deplAsk</t>
-  </si>
-  <si>
     <t>createShapefile</t>
   </si>
   <si>
@@ -202,28 +199,40 @@
     <t>1,2,3,2,1</t>
   </si>
   <si>
+    <t>-20, 60</t>
+  </si>
+  <si>
+    <t>95,50</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>km2</t>
+  </si>
+  <si>
+    <t>coarse</t>
+  </si>
+  <si>
+    <t>kernelStart</t>
+  </si>
+  <si>
+    <t>kernelEnd</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>doTwilights</t>
+  </si>
+  <si>
+    <t>MK3005 050</t>
+  </si>
+  <si>
+    <t>MK3005 050_000.lig</t>
+  </si>
+  <si>
     <t>-80,-40</t>
-  </si>
-  <si>
-    <t>-20, 60</t>
-  </si>
-  <si>
-    <t>95,50</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>km2</t>
-  </si>
-  <si>
-    <t>coarse</t>
-  </si>
-  <si>
-    <t>MK3005 050</t>
-  </si>
-  <si>
-    <t>MK3005 050_000.lig</t>
   </si>
 </sst>
 </file>
@@ -711,10 +720,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -771,10 +782,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1074,69 +1081,72 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BF2"/>
+  <dimension ref="A1:BI5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BG6" sqref="BG6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.85546875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="7" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="57" max="58" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="12.42578125" customWidth="1"/>
+    <col min="52" max="52" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="5" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="60" max="61" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1147,334 +1157,390 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AG1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AH1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AJ1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AL1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AM1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AN1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AO1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AP1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AQ1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AR1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AS1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AT1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AU1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AV1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AW1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AZ1" t="s">
         <v>47</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BA1" t="s">
         <v>48</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BB1" t="s">
         <v>49</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BC1" t="s">
         <v>50</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BD1" t="s">
         <v>51</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BE1" t="s">
         <v>52</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BF1" t="s">
         <v>53</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BG1" t="s">
         <v>54</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BH1" t="s">
         <v>55</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BI1" t="s">
         <v>56</v>
       </c>
-      <c r="BF1" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="2" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B2" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="b">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D2">
+      <c r="E2">
         <v>16</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>5</v>
       </c>
-      <c r="F2" t="b">
+      <c r="G2" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
+      <c r="I2" s="3">
         <v>41524</v>
       </c>
-      <c r="H2" s="1">
+      <c r="J2" s="3">
         <v>41561</v>
       </c>
-      <c r="I2" t="b">
+      <c r="K2" t="b">
         <v>1</v>
       </c>
-      <c r="J2" s="1">
+      <c r="L2" s="3">
         <v>41691</v>
       </c>
-      <c r="K2" s="1">
+      <c r="M2" s="3">
         <v>41736</v>
       </c>
-      <c r="L2" t="b">
+      <c r="N2" t="b">
         <v>1</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="3">
         <v>41493</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="3">
         <v>41791</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="3">
         <v>41493</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="3">
         <v>41791</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>47.257530000000003</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>-52.775568</v>
       </c>
-      <c r="S2" s="2">
+      <c r="U2" s="4">
         <v>41453.625</v>
       </c>
-      <c r="T2" s="2">
+      <c r="V2" s="4">
         <v>41462.625</v>
       </c>
-      <c r="U2">
+      <c r="W2">
         <v>47.257660000000001</v>
       </c>
-      <c r="V2">
+      <c r="X2">
         <v>-52.775759999999998</v>
-      </c>
-      <c r="Z2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AA2" t="b">
-        <v>0</v>
       </c>
       <c r="AB2" t="b">
         <v>0</v>
       </c>
       <c r="AC2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2" t="b">
         <v>1</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" t="b">
         <v>1</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AF2">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH2">
+        <v>5</v>
+      </c>
+      <c r="AI2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>58</v>
-      </c>
-      <c r="AG2">
-        <v>5</v>
-      </c>
-      <c r="AH2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ2" t="b">
-        <v>1</v>
       </c>
       <c r="AK2" t="b">
         <v>1</v>
       </c>
       <c r="AL2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM2" t="b">
         <v>0</v>
       </c>
-      <c r="AM2">
+      <c r="AN2">
         <v>100</v>
       </c>
-      <c r="AN2" t="b">
+      <c r="AO2" t="b">
         <v>1</v>
       </c>
-      <c r="AO2">
+      <c r="AP2">
         <v>-85</v>
       </c>
-      <c r="AP2">
+      <c r="AQ2">
         <v>-30</v>
       </c>
-      <c r="AQ2">
+      <c r="AR2">
         <v>30</v>
       </c>
-      <c r="AR2">
+      <c r="AS2">
         <v>60</v>
       </c>
-      <c r="AS2" t="b">
+      <c r="AT2" t="b">
         <v>0</v>
       </c>
-      <c r="AT2" t="s">
-        <v>60</v>
-      </c>
       <c r="AU2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AV2" t="b">
-        <v>1</v>
+        <v>70</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>59</v>
       </c>
       <c r="AW2" t="b">
         <v>1</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="1"/>
+      <c r="AZ2" t="b">
+        <v>1</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>60</v>
+      </c>
+      <c r="BC2">
+        <v>100000</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>61</v>
+      </c>
+      <c r="BE2" t="s">
         <v>62</v>
       </c>
-      <c r="AZ2">
-        <v>100000</v>
-      </c>
-      <c r="BA2" t="s">
+      <c r="BF2">
+        <v>500</v>
+      </c>
+      <c r="BG2" t="b">
+        <v>1</v>
+      </c>
+      <c r="BH2" t="b">
+        <v>0</v>
+      </c>
+      <c r="BI2" t="s">
         <v>63</v>
       </c>
-      <c r="BB2" t="s">
-        <v>64</v>
-      </c>
-      <c r="BC2">
-        <v>500</v>
-      </c>
-      <c r="BD2" t="b">
-        <v>1</v>
-      </c>
-      <c r="BE2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>65</v>
-      </c>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="1"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="U4" s="2"/>
+      <c r="V4" s="2"/>
+      <c r="AX4" s="1"/>
+      <c r="AY4" s="1"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.25">
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="U5" s="2"/>
+      <c r="V5" s="2"/>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Finish switch to TwGeos::preprocesslight
- also update manual, and distributed config files
- add links to the Geolocation manual to Readme.md and R function docs
</commit_message>
<xml_diff>
--- a/inst/extdata/geolocation_settings.xlsx
+++ b/inst/extdata/geolocation_settings.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://007gc-my.sharepoint.com/personal/dave_fifield_ec_gc_ca/Documents/Projects/__Archived/GLSHelper/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="6_{7BDDE644-5E0F-4C9F-A1B7-CFDF8F32052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDA95808-A6EC-455C-A519-BDE187128DBC}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="6_{7BDDE644-5E0F-4C9F-A1B7-CFDF8F32052B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BCDA959-FDA2-4B5A-B67A-A38FD3AF33B6}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>tagName</t>
   </si>
@@ -34,9 +34,6 @@
     <t>lThresh</t>
   </si>
   <si>
-    <t>maxLightInt</t>
-  </si>
-  <si>
     <t>removeFallEqui</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
     <t>calibLong</t>
   </si>
   <si>
-    <t>calibLThresh</t>
-  </si>
-  <si>
     <t>calibYlim</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>keepCalibPoints</t>
   </si>
   <si>
-    <t>calibAsk</t>
-  </si>
-  <si>
     <t>createShapefile</t>
   </si>
   <si>
@@ -226,13 +217,13 @@
     <t>doTwilights</t>
   </si>
   <si>
-    <t>MK3005 050</t>
-  </si>
-  <si>
     <t>MK3005 050_000.lig</t>
   </si>
   <si>
     <t>-80,-40</t>
+  </si>
+  <si>
+    <t>Mk3005 050</t>
   </si>
 </sst>
 </file>
@@ -1081,72 +1072,69 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BI5"/>
+  <dimension ref="A1:BF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AX1" sqref="AX1"/>
+    <sheetView tabSelected="1" topLeftCell="AX1" workbookViewId="0">
+      <selection activeCell="BF2" sqref="BF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.6328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.08984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.08984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.453125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="15.1796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="11.1796875" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.1796875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="4.1796875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="13" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.36328125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.26953125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.81640625" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="5" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="5" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="5.36328125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="12.36328125" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="9.1796875" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="19.08984375" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="5.26953125" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="5.81640625" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="4" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="60" max="61" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.54296875" customWidth="1"/>
+    <col min="4" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.453125" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="5.453125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="8.26953125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="12.453125" customWidth="1"/>
+    <col min="49" max="49" width="21.1796875" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="7" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="6.26953125" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,16 +1145,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>67</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
@@ -1286,19 +1274,19 @@
         <v>43</v>
       </c>
       <c r="AU1" t="s">
+        <v>61</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>62</v>
+      </c>
+      <c r="AW1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AX1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AY1" t="s">
         <v>46</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>64</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>65</v>
       </c>
       <c r="AZ1" t="s">
         <v>47</v>
@@ -1321,226 +1309,211 @@
       <c r="BF1" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" t="s">
-        <v>54</v>
-      </c>
-      <c r="BH1" t="s">
-        <v>55</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D2" t="b">
         <v>0</v>
       </c>
       <c r="E2">
-        <v>16</v>
-      </c>
-      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="F2" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>41524</v>
+      </c>
+      <c r="I2" s="3">
+        <v>41561</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>41691</v>
+      </c>
+      <c r="L2" s="3">
+        <v>41736</v>
+      </c>
+      <c r="M2" t="b">
+        <v>1</v>
+      </c>
+      <c r="N2" s="3">
+        <v>41493</v>
+      </c>
+      <c r="O2" s="3">
+        <v>41791</v>
+      </c>
+      <c r="P2" s="3">
+        <v>41493</v>
+      </c>
+      <c r="Q2" s="3">
+        <v>41791</v>
+      </c>
+      <c r="R2">
+        <v>47.257530000000003</v>
+      </c>
+      <c r="S2">
+        <v>-52.775568</v>
+      </c>
+      <c r="T2" s="4">
+        <v>41453.625</v>
+      </c>
+      <c r="U2" s="4">
+        <v>41462.625</v>
+      </c>
+      <c r="V2">
+        <v>47.257660000000001</v>
+      </c>
+      <c r="W2">
+        <v>-52.775759999999998</v>
+      </c>
+      <c r="Z2" t="b">
+        <v>0</v>
+      </c>
+      <c r="AA2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE2">
         <v>5</v>
       </c>
-      <c r="G2" t="b">
+      <c r="AF2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AH2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AI2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AJ2" t="b">
         <v>0</v>
       </c>
-      <c r="H2" t="b">
-        <v>1</v>
-      </c>
-      <c r="I2" s="3">
-        <v>41524</v>
-      </c>
-      <c r="J2" s="3">
-        <v>41561</v>
-      </c>
-      <c r="K2" t="b">
-        <v>1</v>
-      </c>
-      <c r="L2" s="3">
-        <v>41691</v>
-      </c>
-      <c r="M2" s="3">
-        <v>41736</v>
-      </c>
-      <c r="N2" t="b">
-        <v>1</v>
-      </c>
-      <c r="O2" s="3">
-        <v>41493</v>
-      </c>
-      <c r="P2" s="3">
-        <v>41791</v>
-      </c>
-      <c r="Q2" s="3">
-        <v>41493</v>
-      </c>
-      <c r="R2" s="3">
-        <v>41791</v>
-      </c>
-      <c r="S2">
-        <v>47.257530000000003</v>
-      </c>
-      <c r="T2">
-        <v>-52.775568</v>
-      </c>
-      <c r="U2" s="4">
-        <v>41453.625</v>
-      </c>
-      <c r="V2" s="4">
-        <v>41462.625</v>
-      </c>
-      <c r="W2">
-        <v>47.257660000000001</v>
-      </c>
-      <c r="X2">
-        <v>-52.775759999999998</v>
-      </c>
-      <c r="AB2" t="b">
+      <c r="AK2">
+        <v>100</v>
+      </c>
+      <c r="AL2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AM2">
+        <v>-85</v>
+      </c>
+      <c r="AN2">
+        <v>-30</v>
+      </c>
+      <c r="AO2">
+        <v>30</v>
+      </c>
+      <c r="AP2">
+        <v>60</v>
+      </c>
+      <c r="AQ2" t="b">
         <v>0</v>
       </c>
-      <c r="AC2" t="b">
+      <c r="AR2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AT2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AU2" s="1"/>
+      <c r="AV2" s="1"/>
+      <c r="AW2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AZ2">
+        <v>100000</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>58</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>59</v>
+      </c>
+      <c r="BC2">
+        <v>500</v>
+      </c>
+      <c r="BD2" t="b">
+        <v>1</v>
+      </c>
+      <c r="BE2" t="b">
         <v>0</v>
       </c>
-      <c r="AD2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AE2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AF2">
-        <v>1</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AH2">
-        <v>5</v>
-      </c>
-      <c r="AI2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AK2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AL2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AM2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AN2">
-        <v>100</v>
-      </c>
-      <c r="AO2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AP2">
-        <v>-85</v>
-      </c>
-      <c r="AQ2">
-        <v>-30</v>
-      </c>
-      <c r="AR2">
-        <v>30</v>
-      </c>
-      <c r="AS2">
+      <c r="BF2" t="s">
         <v>60</v>
       </c>
-      <c r="AT2" t="b">
-        <v>0</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AW2" t="b">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="1"/>
-      <c r="AY2" s="1"/>
-      <c r="AZ2" t="b">
-        <v>1</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>60</v>
-      </c>
-      <c r="BC2">
-        <v>100000</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>61</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>62</v>
-      </c>
-      <c r="BF2">
-        <v>500</v>
-      </c>
-      <c r="BG2" t="b">
-        <v>1</v>
-      </c>
-      <c r="BH2" t="b">
-        <v>0</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>63</v>
-      </c>
     </row>
-    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:58" x14ac:dyDescent="0.35">
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="AX3" s="1"/>
-      <c r="AY3" s="1"/>
+      <c r="AU3" s="1"/>
+      <c r="AV3" s="1"/>
     </row>
-    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:58" x14ac:dyDescent="0.35">
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="AX4" s="1"/>
-      <c r="AY4" s="1"/>
+      <c r="AU4" s="1"/>
+      <c r="AV4" s="1"/>
     </row>
-    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:58" x14ac:dyDescent="0.35">
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
       <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="T5" s="2"/>
       <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="AX5" s="1"/>
-      <c r="AY5" s="1"/>
+      <c r="AU5" s="1"/>
+      <c r="AV5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>